<commit_message>
Report 1 and 2 ready
</commit_message>
<xml_diff>
--- a/MicrotasksReport.xlsx
+++ b/MicrotasksReport.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>File Name</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Explanations</t>
   </si>
   <si>
-    <t>C:\Users\Danilo\Documents\GitHub\crowd-debug-firefly\samples\main\java\com\netflix\nfgraph\util\OrdinalMap_buggy.java</t>
+    <t>OrdinalMap_buggy</t>
   </si>
   <si>
     <t>Is there maybe something wrong in the declaration of function 'growCapacity' at line 128 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
@@ -77,7 +77,7 @@
     <t>Is there perhaps something wrong with the values of the parameters received by function 'copyOf' when called by function 'growCapacity' at line 135 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
   </si>
   <si>
-    <t>C:\Users\Danilo\Documents\GitHub\crowd-debug-firefly\samples\main\java\com\netflix\nfgraph\compressor\CompactPropertyBuilder.java</t>
+    <t>CompactPropertyBuilder</t>
   </si>
   <si>
     <t>Is there maybe something wrong in the declaration of function 'buildProperty' at line 43 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
@@ -122,7 +122,7 @@
     <t>Is there perhaps something wrong with the values of the parameters received by function 'writeVInt' when called by function 'buildProperty' at line 50 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
   </si>
   <si>
-    <t>C:\Users\Danilo\Documents\GitHub\crowd-debug-firefly\samples\main\java\com\netflix\nfgraph\util\ArrayIterator.java</t>
+    <t>ArrayIterator</t>
   </si>
   <si>
     <t>Is there maybe something wrong in the declaration of function 'hasNext' at line 43 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
@@ -177,71 +177,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -366,9 +303,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="114.828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="2.7578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="117.1875" customWidth="true"/>
+    <col min="3" max="3" width="117.1875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="16.984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="58.59375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -382,20 +321,20 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
@@ -406,13 +345,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
@@ -423,13 +362,13 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="n">
         <v>2.0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
@@ -440,13 +379,13 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="n">
         <v>3.0</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
@@ -457,13 +396,13 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="n">
         <v>4.0</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
@@ -474,57 +413,57 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>5.0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="n">
         <v>6.0</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="n">
         <v>7.0</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="n">
         <v>8.0</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="n">
         <v>9.0</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -541,9 +480,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="127.43359375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="23.09375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="2.7578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="117.1875" customWidth="true"/>
+    <col min="3" max="3" width="117.1875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="16.984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="58.59375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -557,20 +498,20 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
@@ -581,13 +522,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D3" t="s">
@@ -598,13 +539,13 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="25" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="n">
         <v>2.0</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
@@ -613,13 +554,13 @@
       <c r="E4"/>
     </row>
     <row r="5">
-      <c r="A5" s="27" t="s">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>3.0</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D5" t="s">
@@ -630,13 +571,13 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="29" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="n">
         <v>4.0</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D6" t="s">
@@ -647,46 +588,46 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="31" t="s">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="n">
         <v>5.0</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="33" t="s">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="n">
         <v>7.0</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="35" t="s">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="n">
         <v>6.0</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="37" t="s">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="n">
         <v>8.0</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="19" t="s">
         <v>34</v>
       </c>
     </row>
@@ -703,9 +644,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="109.390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="12.7265625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="2.7578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="117.1875" customWidth="true"/>
+    <col min="3" max="3" width="117.1875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="16.984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="58.59375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -726,13 +669,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
@@ -743,13 +686,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D3" t="s">

</xml_diff>